<commit_message>
reader friendly format @ xlsx
</commit_message>
<xml_diff>
--- a/fixture/test_fixture.xlsx
+++ b/fixture/test_fixture.xlsx
@@ -76,12 +76,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="hair">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -110,8 +125,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -124,6 +143,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -134,53 +213,53 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L7" activeCellId="0" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.61"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>